<commit_message>
Extract solution for PM2.
</commit_message>
<xml_diff>
--- a/input/input.xlsx
+++ b/input/input.xlsx
@@ -203,10 +203,10 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="4" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -458,15 +458,15 @@
         <v>324.0</v>
       </c>
       <c r="B2" s="2">
-        <v>103.0</v>
-      </c>
-      <c r="C2" s="3">
+        <v>102.7455246</v>
+      </c>
+      <c r="C2" s="2">
         <v>90.0</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2" s="3">
         <v>90.0</v>
       </c>
       <c r="F2" s="4"/>
@@ -476,15 +476,15 @@
         <v>325.0</v>
       </c>
       <c r="B3" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="C3" s="3">
+        <v>55.45854788</v>
+      </c>
+      <c r="C3" s="2">
         <v>50.0</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="3">
         <v>55.0</v>
       </c>
       <c r="F3" s="4"/>
@@ -494,15 +494,15 @@
         <v>326.0</v>
       </c>
       <c r="B4" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C4" s="3">
+        <v>47.25990709</v>
+      </c>
+      <c r="C4" s="2">
         <v>95.0</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4" s="3">
         <v>55.0</v>
       </c>
       <c r="F4" s="4"/>
@@ -512,15 +512,15 @@
         <v>327.0</v>
       </c>
       <c r="B5" s="2">
-        <v>51.0</v>
-      </c>
-      <c r="C5" s="3">
+        <v>50.45854788</v>
+      </c>
+      <c r="C5" s="2">
         <v>45.0</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="3">
         <v>45.0</v>
       </c>
       <c r="F5" s="4"/>
@@ -530,15 +530,15 @@
         <v>328.0</v>
       </c>
       <c r="B6" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C6" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C6" s="2">
         <v>30.0</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6" s="3">
         <v>45.0</v>
       </c>
       <c r="F6" s="4"/>
@@ -548,15 +548,15 @@
         <v>329.0</v>
       </c>
       <c r="B7" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C7" s="3">
+        <v>47.05838099</v>
+      </c>
+      <c r="C7" s="2">
         <v>100.0</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7" s="3">
         <v>34.0</v>
       </c>
       <c r="F7" s="4"/>
@@ -566,15 +566,15 @@
         <v>330.0</v>
       </c>
       <c r="B8" s="2">
-        <v>88.0</v>
-      </c>
-      <c r="C8" s="3">
+        <v>87.36494252</v>
+      </c>
+      <c r="C8" s="2">
         <v>155.0</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8" s="3">
         <v>70.0</v>
       </c>
       <c r="F8" s="4"/>
@@ -584,15 +584,15 @@
         <v>331.0</v>
       </c>
       <c r="B9" s="2">
-        <v>57.0</v>
-      </c>
-      <c r="C9" s="3">
+        <v>56.9476646</v>
+      </c>
+      <c r="C9" s="2">
         <v>95.0</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9" s="3">
         <v>45.0</v>
       </c>
       <c r="F9" s="4"/>
@@ -602,15 +602,15 @@
         <v>332.0</v>
       </c>
       <c r="B10" s="2">
-        <v>43.0</v>
-      </c>
-      <c r="C10" s="3">
+        <v>42.96393105</v>
+      </c>
+      <c r="C10" s="2">
         <v>50.0</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10" s="3">
         <v>30.0</v>
       </c>
       <c r="F10" s="4"/>
@@ -620,15 +620,15 @@
         <v>333.0</v>
       </c>
       <c r="B11" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C11" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C11" s="2">
         <v>60.0</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11" s="3">
         <v>65.0</v>
       </c>
       <c r="F11" s="4"/>
@@ -638,15 +638,15 @@
         <v>334.0</v>
       </c>
       <c r="B12" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C12" s="3">
+        <v>47.05838099</v>
+      </c>
+      <c r="C12" s="2">
         <v>100.0</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12" s="3">
         <v>20.0</v>
       </c>
       <c r="F12" s="4"/>
@@ -656,15 +656,15 @@
         <v>335.0</v>
       </c>
       <c r="B13" s="2">
-        <v>81.0</v>
-      </c>
-      <c r="C13" s="3">
+        <v>80.72346295</v>
+      </c>
+      <c r="C13" s="2">
         <v>135.0</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="3">
         <v>65.0</v>
       </c>
       <c r="F13" s="4"/>
@@ -674,15 +674,15 @@
         <v>336.0</v>
       </c>
       <c r="B14" s="2">
-        <v>99.0</v>
-      </c>
-      <c r="C14" s="3">
+        <v>98.2813512</v>
+      </c>
+      <c r="C14" s="2">
         <v>150.0</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14" s="3">
         <v>115.0</v>
       </c>
       <c r="F14" s="4"/>
@@ -692,15 +692,15 @@
         <v>337.0</v>
       </c>
       <c r="B15" s="2">
-        <v>68.0</v>
-      </c>
-      <c r="C15" s="3">
+        <v>67.23391863</v>
+      </c>
+      <c r="C15" s="2">
         <v>105.0</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15" s="3">
         <v>35.0</v>
       </c>
       <c r="F15" s="4"/>
@@ -710,15 +710,15 @@
         <v>338.0</v>
       </c>
       <c r="B16" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C16" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C16" s="2">
         <v>30.0</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16" s="3">
         <v>30.0</v>
       </c>
       <c r="F16" s="4"/>
@@ -728,15 +728,15 @@
         <v>339.0</v>
       </c>
       <c r="B17" s="2">
-        <v>139.0</v>
-      </c>
-      <c r="C17" s="3">
+        <v>138.0049846</v>
+      </c>
+      <c r="C17" s="2">
         <v>240.0</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="3">
         <v>103.0</v>
       </c>
       <c r="F17" s="4"/>
@@ -746,15 +746,15 @@
         <v>340.0</v>
       </c>
       <c r="B18" s="2">
-        <v>44.0</v>
-      </c>
-      <c r="C18" s="3">
+        <v>43.45545462</v>
+      </c>
+      <c r="C18" s="2">
         <v>50.0</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="3">
         <v>25.0</v>
       </c>
       <c r="F18" s="4"/>
@@ -764,15 +764,15 @@
         <v>341.0</v>
       </c>
       <c r="B19" s="2">
-        <v>44.0</v>
-      </c>
-      <c r="C19" s="3">
+        <v>43.45545462</v>
+      </c>
+      <c r="C19" s="2">
         <v>50.0</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="3">
         <v>40.0</v>
       </c>
       <c r="F19" s="4"/>
@@ -782,15 +782,15 @@
         <v>342.0</v>
       </c>
       <c r="B20" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C20" s="3">
+        <v>47.33170296</v>
+      </c>
+      <c r="C20" s="2">
         <v>40.0</v>
       </c>
       <c r="D20" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20" s="3">
         <v>35.0</v>
       </c>
       <c r="F20" s="4"/>
@@ -800,15 +800,15 @@
         <v>343.0</v>
       </c>
       <c r="B21" s="2">
-        <v>58.0</v>
-      </c>
-      <c r="C21" s="3">
+        <v>57.66374802</v>
+      </c>
+      <c r="C21" s="2">
         <v>130.0</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21" s="3">
         <v>55.0</v>
       </c>
       <c r="F21" s="4"/>
@@ -818,15 +818,15 @@
         <v>344.0</v>
       </c>
       <c r="B22" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="C22" s="3">
+        <v>79.55299783</v>
+      </c>
+      <c r="C22" s="2">
         <v>120.0</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22" s="3">
         <v>85.0</v>
       </c>
       <c r="F22" s="4"/>
@@ -836,15 +836,15 @@
         <v>345.0</v>
       </c>
       <c r="B23" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C23" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C23" s="2">
         <v>60.0</v>
       </c>
       <c r="D23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23" s="3">
         <v>105.0</v>
       </c>
       <c r="F23" s="4"/>
@@ -854,15 +854,15 @@
         <v>346.0</v>
       </c>
       <c r="B24" s="2">
-        <v>52.0</v>
-      </c>
-      <c r="C24" s="3">
+        <v>51.59792481</v>
+      </c>
+      <c r="C24" s="2">
         <v>50.0</v>
       </c>
       <c r="D24" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24" s="3">
         <v>30.0</v>
       </c>
       <c r="F24" s="4"/>
@@ -872,15 +872,15 @@
         <v>347.0</v>
       </c>
       <c r="B25" s="2">
-        <v>47.0</v>
-      </c>
-      <c r="C25" s="3">
+        <v>46.59792481</v>
+      </c>
+      <c r="C25" s="2">
         <v>45.0</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25" s="3">
         <v>35.0</v>
       </c>
       <c r="F25" s="4"/>
@@ -890,15 +890,15 @@
         <v>348.0</v>
       </c>
       <c r="B26" s="2">
-        <v>57.0</v>
-      </c>
-      <c r="C26" s="3">
+        <v>56.78964502</v>
+      </c>
+      <c r="C26" s="2">
         <v>40.0</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26" s="3">
         <v>45.0</v>
       </c>
       <c r="F26" s="4"/>
@@ -908,15 +908,15 @@
         <v>349.0</v>
       </c>
       <c r="B27" s="2">
-        <v>112.0</v>
-      </c>
-      <c r="C27" s="3">
+        <v>111.4641276</v>
+      </c>
+      <c r="C27" s="2">
         <v>240.0</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27" s="3">
         <v>105.0</v>
       </c>
       <c r="F27" s="4"/>
@@ -926,15 +926,15 @@
         <v>350.0</v>
       </c>
       <c r="B28" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C28" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C28" s="2">
         <v>60.0</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28" s="3">
         <v>60.0</v>
       </c>
       <c r="F28" s="4"/>
@@ -944,15 +944,15 @@
         <v>351.0</v>
       </c>
       <c r="B29" s="2">
-        <v>63.0</v>
-      </c>
-      <c r="C29" s="3">
+        <v>62.20699485</v>
+      </c>
+      <c r="C29" s="2">
         <v>60.0</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29" s="3">
         <v>65.0</v>
       </c>
       <c r="F29" s="4"/>
@@ -962,15 +962,15 @@
         <v>352.0</v>
       </c>
       <c r="B30" s="2">
-        <v>52.0</v>
-      </c>
-      <c r="C30" s="3">
+        <v>51.5812351</v>
+      </c>
+      <c r="C30" s="2">
         <v>50.0</v>
       </c>
       <c r="D30" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30" s="3">
         <v>50.0</v>
       </c>
       <c r="F30" s="4"/>
@@ -980,15 +980,15 @@
         <v>353.0</v>
       </c>
       <c r="B31" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C31" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C31" s="2">
         <v>30.0</v>
       </c>
       <c r="D31" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31" s="3">
         <v>35.0</v>
       </c>
       <c r="F31" s="4"/>
@@ -998,15 +998,15 @@
         <v>354.0</v>
       </c>
       <c r="B32" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C32" s="3">
+        <v>47.05838099</v>
+      </c>
+      <c r="C32" s="2">
         <v>100.0</v>
       </c>
       <c r="D32" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32" s="3">
         <v>30.0</v>
       </c>
       <c r="F32" s="4"/>
@@ -1016,15 +1016,15 @@
         <v>355.0</v>
       </c>
       <c r="B33" s="2">
-        <v>51.0</v>
-      </c>
-      <c r="C33" s="3">
+        <v>50.45854788</v>
+      </c>
+      <c r="C33" s="2">
         <v>45.0</v>
       </c>
       <c r="D33" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33" s="3">
         <v>55.0</v>
       </c>
       <c r="F33" s="4"/>
@@ -1034,15 +1034,15 @@
         <v>356.0</v>
       </c>
       <c r="B34" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C34" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C34" s="2">
         <v>60.0</v>
       </c>
       <c r="D34" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34" s="3">
         <v>50.0</v>
       </c>
       <c r="F34" s="4"/>
@@ -1052,15 +1052,15 @@
         <v>357.0</v>
       </c>
       <c r="B35" s="2">
-        <v>118.0</v>
-      </c>
-      <c r="C35" s="3">
+        <v>117.6489211</v>
+      </c>
+      <c r="C35" s="2">
         <v>240.0</v>
       </c>
       <c r="D35" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35" s="3">
         <v>130.0</v>
       </c>
       <c r="F35" s="4"/>
@@ -1070,15 +1070,15 @@
         <v>358.0</v>
       </c>
       <c r="B36" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="C36" s="3">
+        <v>79.27410822</v>
+      </c>
+      <c r="C36" s="2">
         <v>90.0</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36" s="3">
         <v>30.0</v>
       </c>
       <c r="F36" s="4"/>
@@ -1088,15 +1088,15 @@
         <v>359.0</v>
       </c>
       <c r="B37" s="2">
-        <v>110.0</v>
-      </c>
-      <c r="C37" s="3">
+        <v>109.9225551</v>
+      </c>
+      <c r="C37" s="2">
         <v>240.0</v>
       </c>
       <c r="D37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37" s="3">
         <v>105.0</v>
       </c>
       <c r="F37" s="4"/>
@@ -1106,15 +1106,15 @@
         <v>360.0</v>
       </c>
       <c r="B38" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C38" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C38" s="2">
         <v>60.0</v>
       </c>
       <c r="D38" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38" s="3">
         <v>80.0</v>
       </c>
       <c r="F38" s="4"/>
@@ -1124,15 +1124,15 @@
         <v>361.0</v>
       </c>
       <c r="B39" s="2">
-        <v>43.0</v>
-      </c>
-      <c r="C39" s="3">
+        <v>42.96393105</v>
+      </c>
+      <c r="C39" s="2">
         <v>50.0</v>
       </c>
       <c r="D39" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39" s="3">
         <v>75.0</v>
       </c>
       <c r="F39" s="4"/>
@@ -1142,15 +1142,15 @@
         <v>362.0</v>
       </c>
       <c r="B40" s="2">
-        <v>84.0</v>
-      </c>
-      <c r="C40" s="3">
+        <v>83.77549122</v>
+      </c>
+      <c r="C40" s="2">
         <v>120.0</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40" s="3">
         <v>90.0</v>
       </c>
       <c r="F40" s="4"/>
@@ -1160,15 +1160,15 @@
         <v>363.0</v>
       </c>
       <c r="B41" s="2">
-        <v>63.0</v>
-      </c>
-      <c r="C41" s="3">
+        <v>62.20699485</v>
+      </c>
+      <c r="C41" s="2">
         <v>60.0</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41" s="3">
         <v>25.0</v>
       </c>
       <c r="F41" s="4"/>
@@ -1178,15 +1178,15 @@
         <v>364.0</v>
       </c>
       <c r="B42" s="2">
-        <v>50.0</v>
-      </c>
-      <c r="C42" s="3">
+        <v>49.08067193</v>
+      </c>
+      <c r="C42" s="2">
         <v>40.0</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42" s="3">
         <v>40.0</v>
       </c>
       <c r="F42" s="4"/>
@@ -1196,15 +1196,15 @@
         <v>365.0</v>
       </c>
       <c r="B43" s="2">
-        <v>85.0</v>
-      </c>
-      <c r="C43" s="3">
+        <v>84.6954301</v>
+      </c>
+      <c r="C43" s="2">
         <v>210.0</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43" s="3">
         <v>80.0</v>
       </c>
       <c r="F43" s="4"/>
@@ -1214,15 +1214,15 @@
         <v>366.0</v>
       </c>
       <c r="B44" s="2">
-        <v>45.0</v>
-      </c>
-      <c r="C44" s="3">
+        <v>44.45304776</v>
+      </c>
+      <c r="C44" s="2">
         <v>95.0</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44" s="3">
         <v>30.0</v>
       </c>
       <c r="F44" s="4"/>
@@ -1232,15 +1232,15 @@
         <v>367.0</v>
       </c>
       <c r="B45" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="C45" s="3">
+        <v>55.45854788</v>
+      </c>
+      <c r="C45" s="2">
         <v>50.0</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45" s="3">
         <v>45.0</v>
       </c>
       <c r="F45" s="4"/>
@@ -1250,15 +1250,15 @@
         <v>368.0</v>
       </c>
       <c r="B46" s="2">
-        <v>73.0</v>
-      </c>
-      <c r="C46" s="3">
+        <v>72.74713975</v>
+      </c>
+      <c r="C46" s="2">
         <v>60.0</v>
       </c>
       <c r="D46" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46" s="3">
         <v>50.0</v>
       </c>
       <c r="F46" s="4"/>
@@ -1268,15 +1268,15 @@
         <v>369.0</v>
       </c>
       <c r="B47" s="2">
-        <v>80.0</v>
-      </c>
-      <c r="C47" s="3">
+        <v>79.27410822</v>
+      </c>
+      <c r="C47" s="2">
         <v>90.0</v>
       </c>
       <c r="D47" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47" s="3">
         <v>20.0</v>
       </c>
       <c r="F47" s="4"/>
@@ -1286,15 +1286,15 @@
         <v>370.0</v>
       </c>
       <c r="B48" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C48" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C48" s="2">
         <v>60.0</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48" s="3">
         <v>75.0</v>
       </c>
       <c r="F48" s="4"/>
@@ -1304,15 +1304,15 @@
         <v>371.0</v>
       </c>
       <c r="B49" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C49" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C49" s="2">
         <v>30.0</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49" s="3">
         <v>30.0</v>
       </c>
       <c r="F49" s="4"/>
@@ -1322,15 +1322,15 @@
         <v>372.0</v>
       </c>
       <c r="B50" s="2">
-        <v>52.0</v>
-      </c>
-      <c r="C50" s="3">
+        <v>51.28087438</v>
+      </c>
+      <c r="C50" s="2">
         <v>100.0</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50" s="3">
         <v>35.0</v>
       </c>
       <c r="F50" s="4"/>
@@ -1340,15 +1340,15 @@
         <v>373.0</v>
       </c>
       <c r="B51" s="2">
-        <v>41.0</v>
-      </c>
-      <c r="C51" s="3">
+        <v>40.64488056</v>
+      </c>
+      <c r="C51" s="2">
         <v>50.0</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51" s="3">
         <v>25.0</v>
       </c>
       <c r="F51" s="4"/>
@@ -1358,15 +1358,15 @@
         <v>374.0</v>
       </c>
       <c r="B52" s="2">
-        <v>60.0</v>
-      </c>
-      <c r="C52" s="3">
+        <v>59.03844493</v>
+      </c>
+      <c r="C52" s="2">
         <v>100.0</v>
       </c>
       <c r="D52" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52" s="3">
         <v>40.0</v>
       </c>
       <c r="F52" s="4"/>
@@ -1376,15 +1376,15 @@
         <v>375.0</v>
       </c>
       <c r="B53" s="2">
-        <v>48.0</v>
-      </c>
-      <c r="C53" s="3">
+        <v>47.33170296</v>
+      </c>
+      <c r="C53" s="2">
         <v>40.0</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53" s="3">
         <v>35.0</v>
       </c>
       <c r="F53" s="4"/>
@@ -1394,15 +1394,15 @@
         <v>376.0</v>
       </c>
       <c r="B54" s="2">
-        <v>44.0</v>
-      </c>
-      <c r="C54" s="3">
+        <v>43.35202748</v>
+      </c>
+      <c r="C54" s="2">
         <v>50.0</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54" s="3">
         <v>25.0</v>
       </c>
       <c r="F54" s="4"/>
@@ -1412,15 +1412,15 @@
         <v>377.0</v>
       </c>
       <c r="B55" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C55" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C55" s="2">
         <v>30.0</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55" s="3">
         <v>30.0</v>
       </c>
       <c r="F55" s="4"/>
@@ -1430,15 +1430,15 @@
         <v>378.0</v>
       </c>
       <c r="B56" s="2">
-        <v>41.0</v>
-      </c>
-      <c r="C56" s="3">
+        <v>40.64488056</v>
+      </c>
+      <c r="C56" s="2">
         <v>50.0</v>
       </c>
       <c r="D56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56" s="3">
         <v>30.0</v>
       </c>
       <c r="F56" s="4"/>
@@ -1448,15 +1448,15 @@
         <v>379.0</v>
       </c>
       <c r="B57" s="2">
-        <v>43.0</v>
-      </c>
-      <c r="C57" s="3">
+        <v>42.32133471</v>
+      </c>
+      <c r="C57" s="2">
         <v>100.0</v>
       </c>
       <c r="D57" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57" s="3">
         <v>35.0</v>
       </c>
       <c r="F57" s="4"/>
@@ -1466,15 +1466,15 @@
         <v>380.0</v>
       </c>
       <c r="B58" s="2">
-        <v>41.0</v>
-      </c>
-      <c r="C58" s="3">
+        <v>40.64488056</v>
+      </c>
+      <c r="C58" s="2">
         <v>50.0</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58" s="3">
         <v>25.0</v>
       </c>
       <c r="F58" s="4"/>
@@ -1484,15 +1484,15 @@
         <v>381.0</v>
       </c>
       <c r="B59" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C59" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C59" s="2">
         <v>30.0</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59" s="3">
         <v>55.0</v>
       </c>
       <c r="F59" s="4"/>
@@ -1502,15 +1502,15 @@
         <v>382.0</v>
       </c>
       <c r="B60" s="2">
-        <v>62.0</v>
-      </c>
-      <c r="C60" s="3">
+        <v>61.28087438</v>
+      </c>
+      <c r="C60" s="2">
         <v>110.0</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60" s="3">
         <v>50.0</v>
       </c>
       <c r="F60" s="4"/>
@@ -1520,15 +1520,15 @@
         <v>383.0</v>
       </c>
       <c r="B61" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="C61" s="3">
+        <v>55.45854788</v>
+      </c>
+      <c r="C61" s="2">
         <v>50.0</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61" s="3">
         <v>35.0</v>
       </c>
       <c r="F61" s="4"/>
@@ -1538,15 +1538,15 @@
         <v>384.0</v>
       </c>
       <c r="B62" s="2">
-        <v>118.0</v>
-      </c>
-      <c r="C62" s="3">
+        <v>117.6489211</v>
+      </c>
+      <c r="C62" s="2">
         <v>240.0</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62" s="3">
         <v>110.0</v>
       </c>
       <c r="F62" s="4"/>
@@ -1556,15 +1556,15 @@
         <v>385.0</v>
       </c>
       <c r="B63" s="2">
-        <v>56.0</v>
-      </c>
-      <c r="C63" s="3">
+        <v>55.45854788</v>
+      </c>
+      <c r="C63" s="2">
         <v>50.0</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63" s="3">
         <v>40.0</v>
       </c>
       <c r="F63" s="4"/>
@@ -1574,15 +1574,15 @@
         <v>386.0</v>
       </c>
       <c r="B64" s="2">
-        <v>68.0</v>
-      </c>
-      <c r="C64" s="3">
+        <v>67.96265791</v>
+      </c>
+      <c r="C64" s="2">
         <v>110.0</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64" s="3">
         <v>30.0</v>
       </c>
       <c r="F64" s="4"/>
@@ -1592,15 +1592,15 @@
         <v>387.0</v>
       </c>
       <c r="B65" s="2">
-        <v>92.0</v>
-      </c>
-      <c r="C65" s="3">
+        <v>91.76872506</v>
+      </c>
+      <c r="C65" s="2">
         <v>90.0</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65" s="3">
         <v>70.0</v>
       </c>
       <c r="F65" s="4"/>
@@ -1610,15 +1610,15 @@
         <v>388.0</v>
       </c>
       <c r="B66" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C66" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C66" s="2">
         <v>60.0</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66" s="3">
         <v>55.0</v>
       </c>
       <c r="F66" s="4"/>
@@ -1628,15 +1628,15 @@
         <v>389.0</v>
       </c>
       <c r="B67" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C67" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C67" s="2">
         <v>30.0</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67" s="3">
         <v>45.0</v>
       </c>
       <c r="F67" s="4"/>
@@ -1646,15 +1646,15 @@
         <v>390.0</v>
       </c>
       <c r="B68" s="2">
-        <v>74.0</v>
-      </c>
-      <c r="C68" s="3">
+        <v>73.77549122</v>
+      </c>
+      <c r="C68" s="2">
         <v>110.0</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68" s="3">
         <v>60.0</v>
       </c>
       <c r="F68" s="4"/>
@@ -1664,15 +1664,15 @@
         <v>391.0</v>
       </c>
       <c r="B69" s="2">
-        <v>74.0</v>
-      </c>
-      <c r="C69" s="3">
+        <v>73.77549122</v>
+      </c>
+      <c r="C69" s="2">
         <v>110.0</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69" s="3">
         <v>60.0</v>
       </c>
       <c r="F69" s="4"/>
@@ -1682,15 +1682,15 @@
         <v>392.0</v>
       </c>
       <c r="B70" s="2">
-        <v>73.0</v>
-      </c>
-      <c r="C70" s="3">
+        <v>72.23391863</v>
+      </c>
+      <c r="C70" s="2">
         <v>110.0</v>
       </c>
       <c r="D70" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70" s="3">
         <v>85.0</v>
       </c>
       <c r="F70" s="4"/>
@@ -1700,15 +1700,15 @@
         <v>393.0</v>
       </c>
       <c r="B71" s="2">
-        <v>66.0</v>
-      </c>
-      <c r="C71" s="3">
+        <v>65.45854788</v>
+      </c>
+      <c r="C71" s="2">
         <v>60.0</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71" s="3">
         <v>55.0</v>
       </c>
       <c r="F71" s="4"/>
@@ -1718,15 +1718,15 @@
         <v>394.0</v>
       </c>
       <c r="B72" s="2">
-        <v>42.0</v>
-      </c>
-      <c r="C72" s="3">
+        <v>41.603785</v>
+      </c>
+      <c r="C72" s="2">
         <v>50.0</v>
       </c>
       <c r="D72" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72" s="3">
         <v>35.0</v>
       </c>
       <c r="F72" s="4"/>
@@ -1736,15 +1736,15 @@
         <v>395.0</v>
       </c>
       <c r="B73" s="2">
-        <v>65.0</v>
-      </c>
-      <c r="C73" s="3">
+        <v>64.09840184</v>
+      </c>
+      <c r="C73" s="2">
         <v>60.0</v>
       </c>
       <c r="D73" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73" s="3">
         <v>45.0</v>
       </c>
       <c r="F73" s="4"/>
@@ -1754,15 +1754,15 @@
         <v>396.0</v>
       </c>
       <c r="B74" s="2">
-        <v>120.0</v>
-      </c>
-      <c r="C74" s="3">
+        <v>119.9641002</v>
+      </c>
+      <c r="C74" s="2">
         <v>240.0</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74" s="3">
         <v>95.0</v>
       </c>
       <c r="F74" s="4"/>
@@ -1772,15 +1772,15 @@
         <v>397.0</v>
       </c>
       <c r="B75" s="2">
-        <v>70.0</v>
-      </c>
-      <c r="C75" s="3">
+        <v>69.27410822</v>
+      </c>
+      <c r="C75" s="2">
         <v>80.0</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75" s="3">
         <v>40.0</v>
       </c>
       <c r="F75" s="4"/>
@@ -1790,15 +1790,15 @@
         <v>398.0</v>
       </c>
       <c r="B76" s="2">
-        <v>62.0</v>
-      </c>
-      <c r="C76" s="3">
+        <v>61.28087438</v>
+      </c>
+      <c r="C76" s="2">
         <v>110.0</v>
       </c>
       <c r="D76" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76" s="3">
         <v>35.0</v>
       </c>
       <c r="F76" s="4"/>
@@ -1808,15 +1808,15 @@
         <v>399.0</v>
       </c>
       <c r="B77" s="2">
-        <v>40.0</v>
-      </c>
-      <c r="C77" s="3">
+        <v>39.08067193</v>
+      </c>
+      <c r="C77" s="2">
         <v>30.0</v>
       </c>
       <c r="D77" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77" s="3">
         <v>20.0</v>
       </c>
       <c r="F77" s="4"/>

</xml_diff>